<commit_message>
hecho pero sin funcionar bien del todo
</commit_message>
<xml_diff>
--- a/resources/SistemasVehiculos.xlsx
+++ b/resources/SistemasVehiculos.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1251" uniqueCount="658">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1433" uniqueCount="831">
   <si>
     <t>Nombre</t>
   </si>
@@ -2000,6 +2000,525 @@
   </si>
   <si>
     <t>215465</t>
+  </si>
+  <si>
+    <t>ES1220125003305201112544</t>
+  </si>
+  <si>
+    <t>vdo00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES2821651484690980008984</t>
+  </si>
+  <si>
+    <t>vbp00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES3520960043043554600000</t>
+  </si>
+  <si>
+    <t>abp00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES7921564975243245467995</t>
+  </si>
+  <si>
+    <t>map00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES4932566221522587754554</t>
+  </si>
+  <si>
+    <t>acp00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES2500750184310702510000</t>
+  </si>
+  <si>
+    <t>agp00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES7025894363435485700142</t>
+  </si>
+  <si>
+    <t>lbr00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES4896431245148150005176</t>
+  </si>
+  <si>
+    <t>sbr00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES3525030000114574745458</t>
+  </si>
+  <si>
+    <t>agr00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES3115953684811254695203</t>
+  </si>
+  <si>
+    <t>dgr00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES9020960043023096200000</t>
+  </si>
+  <si>
+    <t>pgs00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>cis00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES5023455254943263234457</t>
+  </si>
+  <si>
+    <t>mqf00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES6420910936583000000000</t>
+  </si>
+  <si>
+    <t>bvm00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES3720960043032159000000</t>
+  </si>
+  <si>
+    <t>ppr00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES0412669681115112121210</t>
+  </si>
+  <si>
+    <t>pcs00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES2956187775315550000651</t>
+  </si>
+  <si>
+    <t>gmm00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES0425516848021156151054</t>
+  </si>
+  <si>
+    <t>cgm00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES6264578946740051516490</t>
+  </si>
+  <si>
+    <t>gmm01@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES4534698752714600549403</t>
+  </si>
+  <si>
+    <t>csn00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES2766649444162310000255</t>
+  </si>
+  <si>
+    <t>alo00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES6223185484465641685100</t>
+  </si>
+  <si>
+    <t>gmm02@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES9621508149175421346497</t>
+  </si>
+  <si>
+    <t>tcp00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES1621346154503164978451</t>
+  </si>
+  <si>
+    <t>ccp00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES7225187786311225455548</t>
+  </si>
+  <si>
+    <t>cap00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES4723164897642213030615</t>
+  </si>
+  <si>
+    <t>sfp00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES2396536214865214585214</t>
+  </si>
+  <si>
+    <t>elr00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES6885461325251978750005</t>
+  </si>
+  <si>
+    <t>dlr00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES2924587946032003165464</t>
+  </si>
+  <si>
+    <t>har00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES5020960043073071400000</t>
+  </si>
+  <si>
+    <t>spr00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES8220960043042158800000</t>
+  </si>
+  <si>
+    <t>gpr00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES7521654587985156484454</t>
+  </si>
+  <si>
+    <t>sas00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES3251651681961210656510</t>
+  </si>
+  <si>
+    <t>bfs00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES5566552211148855332200</t>
+  </si>
+  <si>
+    <t>dfg00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>gmg00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES4201821135910205540000</t>
+  </si>
+  <si>
+    <t>mlg00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES2722631245526916432102</t>
+  </si>
+  <si>
+    <t>iag00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES2120960043043075700000</t>
+  </si>
+  <si>
+    <t>iag01@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES8425635478321002541225</t>
+  </si>
+  <si>
+    <t>gpg00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES6832154697195423121000</t>
+  </si>
+  <si>
+    <t>rgg00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES5336521452736500658485</t>
+  </si>
+  <si>
+    <t>apg00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES2220008521528775113366</t>
+  </si>
+  <si>
+    <t>afg00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES8020960043033000100000</t>
+  </si>
+  <si>
+    <t>apm00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES7236585214290025478551</t>
+  </si>
+  <si>
+    <t>gmm03@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES9012548523465214585214</t>
+  </si>
+  <si>
+    <t>alm00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES6931624561042546920007</t>
+  </si>
+  <si>
+    <t>ldm00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES1436154231712500312566</t>
+  </si>
+  <si>
+    <t>adg00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES8244875664127231645789</t>
+  </si>
+  <si>
+    <t>lrf00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES7920960031442124800000</t>
+  </si>
+  <si>
+    <t>lcg00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES1633620012937852100256</t>
+  </si>
+  <si>
+    <t>sbg00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES1933218885441445121022</t>
+  </si>
+  <si>
+    <t>afg01@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES8462581542713690044508</t>
+  </si>
+  <si>
+    <t>dgg00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES3925165151118666365100</t>
+  </si>
+  <si>
+    <t>rog00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>sog00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES4036952365020014425254</t>
+  </si>
+  <si>
+    <t>vvg00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES9565168874641561561500</t>
+  </si>
+  <si>
+    <t>vmg00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES3220960583831234500000</t>
+  </si>
+  <si>
+    <t>mbg00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES7221416325811510005514</t>
+  </si>
+  <si>
+    <t>cbg00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES7832628484504115151115</t>
+  </si>
+  <si>
+    <t>msh00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES2220960056133231500000</t>
+  </si>
+  <si>
+    <t>fdl00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES8163516541828944000984</t>
+  </si>
+  <si>
+    <t>sdm00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES6223658965274585223202</t>
+  </si>
+  <si>
+    <t>egm00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES4032658012367712548745</t>
+  </si>
+  <si>
+    <t>gpm00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES7223652365142254222000</t>
+  </si>
+  <si>
+    <t>eam00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES4420012541150023365233</t>
+  </si>
+  <si>
+    <t>mmm00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES9232584216971684051000</t>
+  </si>
+  <si>
+    <t>mgf00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES7395485212315484010000</t>
+  </si>
+  <si>
+    <t>jac00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES6221856333126985542360</t>
+  </si>
+  <si>
+    <t>bdc00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES5736245978133245679001</t>
+  </si>
+  <si>
+    <t>ngc00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES7631245164156597845124</t>
+  </si>
+  <si>
+    <t>mlc00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES5523221158252545471411</t>
+  </si>
+  <si>
+    <t>mhg00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES5532574512085411002255</t>
+  </si>
+  <si>
+    <t>mlc01@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES4420960043013468900000</t>
+  </si>
+  <si>
+    <t>cfc00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES5631215643855060225021</t>
+  </si>
+  <si>
+    <t>cgc00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES9685550564726165145610</t>
+  </si>
+  <si>
+    <t>hsc00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES1665165654918886005001</t>
+  </si>
+  <si>
+    <t>ksc00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES5065645150865168448896</t>
+  </si>
+  <si>
+    <t>mhc00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES7426551681807651415636</t>
+  </si>
+  <si>
+    <t>cld00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES5699558741836555551120</t>
+  </si>
+  <si>
+    <t>mfd00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES4352198484752100515144</t>
+  </si>
+  <si>
+    <t>fgd00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES6251556584221251000254</t>
+  </si>
+  <si>
+    <t>gmm04@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES5732541112811220000588</t>
+  </si>
+  <si>
+    <t>ivc00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES6262541122421110105611</t>
+  </si>
+  <si>
+    <t>dmc00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ebc00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>nbc00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>msc00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>mdc00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>mfc00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>cdd00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES9836250012804785523365</t>
+  </si>
+  <si>
+    <t>cgd00@vehiculos2025.com</t>
+  </si>
+  <si>
+    <t>ES9522515651915640081000</t>
+  </si>
+  <si>
+    <t>hpd00@vehiculos2025.com</t>
   </si>
 </sst>
 </file>
@@ -2639,6 +3158,9 @@
       <c r="F8" s="6" t="s">
         <v>294</v>
       </c>
+      <c r="G8" t="s" s="0">
+        <v>659</v>
+      </c>
       <c r="H8" t="s" s="0">
         <v>550</v>
       </c>
@@ -2647,6 +3169,9 @@
       </c>
       <c r="J8" s="3" t="s">
         <v>144</v>
+      </c>
+      <c r="K8" t="s">
+        <v>658</v>
       </c>
       <c r="L8" s="0">
         <v>0</v>
@@ -2671,6 +3196,9 @@
       <c r="F9" s="6" t="s">
         <v>294</v>
       </c>
+      <c r="G9" t="s" s="0">
+        <v>661</v>
+      </c>
       <c r="H9" t="s" s="0">
         <v>550</v>
       </c>
@@ -2679,6 +3207,9 @@
       </c>
       <c r="J9" s="3" t="s">
         <v>145</v>
+      </c>
+      <c r="K9" t="s">
+        <v>660</v>
       </c>
       <c r="L9" s="0">
         <v>0</v>
@@ -2703,6 +3234,9 @@
       <c r="F10" s="6" t="s">
         <v>295</v>
       </c>
+      <c r="G10" t="s" s="0">
+        <v>663</v>
+      </c>
       <c r="H10" t="s" s="0">
         <v>550</v>
       </c>
@@ -2711,6 +3245,9 @@
       </c>
       <c r="J10" s="3" t="s">
         <v>146</v>
+      </c>
+      <c r="K10" t="s">
+        <v>662</v>
       </c>
       <c r="L10" s="0">
         <v>0</v>
@@ -2735,6 +3272,9 @@
       <c r="F11" s="6" t="s">
         <v>296</v>
       </c>
+      <c r="G11" t="s" s="0">
+        <v>665</v>
+      </c>
       <c r="H11" t="s" s="0">
         <v>550</v>
       </c>
@@ -2743,6 +3283,9 @@
       </c>
       <c r="J11" s="3" t="s">
         <v>147</v>
+      </c>
+      <c r="K11" t="s">
+        <v>664</v>
       </c>
       <c r="L11" s="0">
         <v>0</v>
@@ -2767,6 +3310,9 @@
       <c r="F12" s="6" t="s">
         <v>296</v>
       </c>
+      <c r="G12" t="s" s="0">
+        <v>667</v>
+      </c>
       <c r="H12" t="s" s="0">
         <v>550</v>
       </c>
@@ -2775,6 +3321,9 @@
       </c>
       <c r="J12" s="3" t="s">
         <v>148</v>
+      </c>
+      <c r="K12" t="s">
+        <v>666</v>
       </c>
       <c r="L12" s="0">
         <v>0</v>
@@ -2829,6 +3378,9 @@
       <c r="F14" s="6" t="s">
         <v>297</v>
       </c>
+      <c r="G14" t="s" s="0">
+        <v>669</v>
+      </c>
       <c r="H14" t="s" s="0">
         <v>550</v>
       </c>
@@ -2837,6 +3389,9 @@
       </c>
       <c r="J14" s="3" t="s">
         <v>150</v>
+      </c>
+      <c r="K14" t="s">
+        <v>668</v>
       </c>
       <c r="L14" s="0">
         <v>0</v>
@@ -2867,6 +3422,9 @@
       <c r="F16" s="6" t="s">
         <v>299</v>
       </c>
+      <c r="G16" t="s" s="0">
+        <v>671</v>
+      </c>
       <c r="H16" t="s" s="0">
         <v>550</v>
       </c>
@@ -2875,6 +3433,9 @@
       </c>
       <c r="J16" s="3" t="s">
         <v>645</v>
+      </c>
+      <c r="K16" t="s">
+        <v>670</v>
       </c>
       <c r="L16" s="0">
         <v>0</v>
@@ -2899,6 +3460,9 @@
       <c r="F17" s="6" t="s">
         <v>300</v>
       </c>
+      <c r="G17" t="s" s="0">
+        <v>673</v>
+      </c>
       <c r="H17" t="s" s="0">
         <v>550</v>
       </c>
@@ -2907,6 +3471,9 @@
       </c>
       <c r="J17" s="3" t="s">
         <v>646</v>
+      </c>
+      <c r="K17" t="s">
+        <v>672</v>
       </c>
       <c r="L17" s="0">
         <v>0</v>
@@ -2931,6 +3498,9 @@
       <c r="F18" s="6" t="s">
         <v>300</v>
       </c>
+      <c r="G18" t="s" s="0">
+        <v>675</v>
+      </c>
       <c r="H18" t="s" s="0">
         <v>550</v>
       </c>
@@ -2939,6 +3509,9 @@
       </c>
       <c r="J18" s="3" t="s">
         <v>151</v>
+      </c>
+      <c r="K18" t="s">
+        <v>674</v>
       </c>
       <c r="L18" s="0">
         <v>0</v>
@@ -2963,6 +3536,9 @@
       <c r="F19" s="6" t="s">
         <v>299</v>
       </c>
+      <c r="G19" t="s" s="0">
+        <v>677</v>
+      </c>
       <c r="H19" t="s" s="0">
         <v>550</v>
       </c>
@@ -2971,6 +3547,9 @@
       </c>
       <c r="J19" s="3" t="s">
         <v>152</v>
+      </c>
+      <c r="K19" t="s">
+        <v>676</v>
       </c>
       <c r="L19" s="0">
         <v>0</v>
@@ -2995,6 +3574,9 @@
       <c r="F20" s="6" t="s">
         <v>299</v>
       </c>
+      <c r="G20" t="s" s="0">
+        <v>679</v>
+      </c>
       <c r="H20" t="s" s="0">
         <v>550</v>
       </c>
@@ -3003,6 +3585,9 @@
       </c>
       <c r="J20" s="3" t="s">
         <v>153</v>
+      </c>
+      <c r="K20" t="s">
+        <v>678</v>
       </c>
       <c r="L20" s="0">
         <v>0</v>
@@ -3027,6 +3612,9 @@
       <c r="F21" s="6" t="s">
         <v>300</v>
       </c>
+      <c r="G21" t="s" s="0">
+        <v>680</v>
+      </c>
       <c r="H21" t="s" s="0">
         <v>550</v>
       </c>
@@ -3035,6 +3623,9 @@
       </c>
       <c r="J21" s="3" t="s">
         <v>150</v>
+      </c>
+      <c r="K21" t="s">
+        <v>668</v>
       </c>
       <c r="L21" s="0">
         <v>0</v>
@@ -3059,6 +3650,9 @@
       <c r="F22" s="6" t="s">
         <v>301</v>
       </c>
+      <c r="G22" t="s" s="0">
+        <v>682</v>
+      </c>
       <c r="H22" t="s" s="0">
         <v>550</v>
       </c>
@@ -3067,6 +3661,9 @@
       </c>
       <c r="J22" s="3" t="s">
         <v>154</v>
+      </c>
+      <c r="K22" t="s">
+        <v>681</v>
       </c>
       <c r="L22" s="0">
         <v>0</v>
@@ -3091,6 +3688,9 @@
       <c r="F23" s="6" t="s">
         <v>302</v>
       </c>
+      <c r="G23" t="s" s="0">
+        <v>684</v>
+      </c>
       <c r="H23" t="s" s="0">
         <v>550</v>
       </c>
@@ -3099,6 +3699,9 @@
       </c>
       <c r="J23" s="3" t="s">
         <v>155</v>
+      </c>
+      <c r="K23" t="s">
+        <v>683</v>
       </c>
       <c r="L23" s="0">
         <v>0</v>
@@ -3123,6 +3726,9 @@
       <c r="F24" s="6" t="s">
         <v>300</v>
       </c>
+      <c r="G24" t="s" s="0">
+        <v>686</v>
+      </c>
       <c r="H24" t="s" s="0">
         <v>550</v>
       </c>
@@ -3131,6 +3737,9 @@
       </c>
       <c r="J24" s="3" t="s">
         <v>156</v>
+      </c>
+      <c r="K24" t="s">
+        <v>685</v>
       </c>
       <c r="L24" s="0">
         <v>0</v>
@@ -3155,6 +3764,9 @@
       <c r="F25" s="6" t="s">
         <v>303</v>
       </c>
+      <c r="G25" t="s" s="0">
+        <v>688</v>
+      </c>
       <c r="H25" t="s" s="0">
         <v>550</v>
       </c>
@@ -3163,6 +3775,9 @@
       </c>
       <c r="J25" s="3" t="s">
         <v>157</v>
+      </c>
+      <c r="K25" t="s">
+        <v>687</v>
       </c>
       <c r="L25" s="0">
         <v>0</v>
@@ -3193,6 +3808,9 @@
       <c r="F27" s="6" t="s">
         <v>300</v>
       </c>
+      <c r="G27" t="s" s="0">
+        <v>690</v>
+      </c>
       <c r="H27" t="s" s="0">
         <v>550</v>
       </c>
@@ -3201,6 +3819,9 @@
       </c>
       <c r="J27" s="3" t="s">
         <v>158</v>
+      </c>
+      <c r="K27" t="s">
+        <v>689</v>
       </c>
       <c r="L27" s="0">
         <v>0</v>
@@ -3225,6 +3846,9 @@
       <c r="F28" s="6" t="s">
         <v>293</v>
       </c>
+      <c r="G28" t="s" s="0">
+        <v>692</v>
+      </c>
       <c r="H28" t="s" s="0">
         <v>550</v>
       </c>
@@ -3233,6 +3857,9 @@
       </c>
       <c r="J28" s="3" t="s">
         <v>159</v>
+      </c>
+      <c r="K28" t="s">
+        <v>691</v>
       </c>
       <c r="L28" s="0">
         <v>0</v>
@@ -3257,6 +3884,9 @@
       <c r="F29" s="6" t="s">
         <v>297</v>
       </c>
+      <c r="G29" t="s" s="0">
+        <v>694</v>
+      </c>
       <c r="H29" t="s" s="0">
         <v>550</v>
       </c>
@@ -3265,6 +3895,9 @@
       </c>
       <c r="J29" s="3" t="s">
         <v>160</v>
+      </c>
+      <c r="K29" t="s">
+        <v>693</v>
       </c>
       <c r="L29" s="0">
         <v>0</v>
@@ -3289,6 +3922,9 @@
       <c r="F30" s="6" t="s">
         <v>297</v>
       </c>
+      <c r="G30" t="s" s="0">
+        <v>696</v>
+      </c>
       <c r="H30" t="s" s="0">
         <v>550</v>
       </c>
@@ -3297,6 +3933,9 @@
       </c>
       <c r="J30" s="3" t="s">
         <v>161</v>
+      </c>
+      <c r="K30" t="s">
+        <v>695</v>
       </c>
       <c r="L30" s="0">
         <v>0</v>
@@ -3321,6 +3960,9 @@
       <c r="F31" s="6" t="s">
         <v>297</v>
       </c>
+      <c r="G31" t="s" s="0">
+        <v>698</v>
+      </c>
       <c r="H31" t="s" s="0">
         <v>550</v>
       </c>
@@ -3329,6 +3971,9 @@
       </c>
       <c r="J31" s="3" t="s">
         <v>162</v>
+      </c>
+      <c r="K31" t="s">
+        <v>697</v>
       </c>
       <c r="L31" s="0">
         <v>0</v>
@@ -3353,6 +3998,9 @@
       <c r="F32" s="6" t="s">
         <v>304</v>
       </c>
+      <c r="G32" t="s" s="0">
+        <v>700</v>
+      </c>
       <c r="H32" t="s" s="0">
         <v>550</v>
       </c>
@@ -3361,6 +4009,9 @@
       </c>
       <c r="J32" s="3" t="s">
         <v>163</v>
+      </c>
+      <c r="K32" t="s">
+        <v>699</v>
       </c>
       <c r="L32" s="0">
         <v>0</v>
@@ -3403,6 +4054,9 @@
       <c r="F36" s="6" t="s">
         <v>302</v>
       </c>
+      <c r="G36" t="s" s="0">
+        <v>702</v>
+      </c>
       <c r="H36" t="s" s="0">
         <v>550</v>
       </c>
@@ -3411,6 +4065,9 @@
       </c>
       <c r="J36" s="3" t="s">
         <v>164</v>
+      </c>
+      <c r="K36" t="s">
+        <v>701</v>
       </c>
       <c r="L36" s="0">
         <v>0</v>
@@ -3435,6 +4092,9 @@
       <c r="F37" s="6" t="s">
         <v>290</v>
       </c>
+      <c r="G37" t="s" s="0">
+        <v>704</v>
+      </c>
       <c r="H37" t="s" s="0">
         <v>550</v>
       </c>
@@ -3443,6 +4103,9 @@
       </c>
       <c r="J37" s="3" t="s">
         <v>165</v>
+      </c>
+      <c r="K37" t="s">
+        <v>703</v>
       </c>
       <c r="L37" s="0">
         <v>0</v>
@@ -3467,6 +4130,9 @@
       <c r="F38" s="6" t="s">
         <v>301</v>
       </c>
+      <c r="G38" t="s" s="0">
+        <v>706</v>
+      </c>
       <c r="H38" t="s" s="0">
         <v>550</v>
       </c>
@@ -3475,6 +4141,9 @@
       </c>
       <c r="J38" s="3" t="s">
         <v>166</v>
+      </c>
+      <c r="K38" t="s">
+        <v>705</v>
       </c>
       <c r="L38" s="0">
         <v>0</v>
@@ -3499,6 +4168,9 @@
       <c r="F39" s="6" t="s">
         <v>306</v>
       </c>
+      <c r="G39" t="s" s="0">
+        <v>708</v>
+      </c>
       <c r="H39" t="s" s="0">
         <v>550</v>
       </c>
@@ -3507,6 +4179,9 @@
       </c>
       <c r="J39" s="3" t="s">
         <v>167</v>
+      </c>
+      <c r="K39" t="s">
+        <v>707</v>
       </c>
       <c r="L39" s="0">
         <v>0</v>
@@ -3531,6 +4206,9 @@
       <c r="F40" s="6" t="s">
         <v>307</v>
       </c>
+      <c r="G40" t="s" s="0">
+        <v>710</v>
+      </c>
       <c r="H40" t="s" s="0">
         <v>550</v>
       </c>
@@ -3539,6 +4217,9 @@
       </c>
       <c r="J40" s="3" t="s">
         <v>168</v>
+      </c>
+      <c r="K40" t="s">
+        <v>709</v>
       </c>
       <c r="L40" s="0">
         <v>0</v>
@@ -3563,6 +4244,9 @@
       <c r="F41" s="6" t="s">
         <v>307</v>
       </c>
+      <c r="G41" t="s" s="0">
+        <v>712</v>
+      </c>
       <c r="H41" t="s" s="0">
         <v>550</v>
       </c>
@@ -3571,6 +4255,9 @@
       </c>
       <c r="J41" s="3" t="s">
         <v>169</v>
+      </c>
+      <c r="K41" t="s">
+        <v>711</v>
       </c>
       <c r="L41" s="0">
         <v>0</v>
@@ -3595,6 +4282,9 @@
       <c r="F42" s="6" t="s">
         <v>307</v>
       </c>
+      <c r="G42" t="s" s="0">
+        <v>714</v>
+      </c>
       <c r="H42" t="s" s="0">
         <v>550</v>
       </c>
@@ -3603,6 +4293,9 @@
       </c>
       <c r="J42" s="3" t="s">
         <v>170</v>
+      </c>
+      <c r="K42" t="s">
+        <v>713</v>
       </c>
       <c r="L42" s="0">
         <v>0</v>
@@ -3627,6 +4320,9 @@
       <c r="F43" s="6" t="s">
         <v>308</v>
       </c>
+      <c r="G43" t="s" s="0">
+        <v>716</v>
+      </c>
       <c r="H43" t="s" s="0">
         <v>550</v>
       </c>
@@ -3635,6 +4331,9 @@
       </c>
       <c r="J43" s="3" t="s">
         <v>171</v>
+      </c>
+      <c r="K43" t="s">
+        <v>715</v>
       </c>
       <c r="L43" s="0">
         <v>0</v>
@@ -3659,6 +4358,9 @@
       <c r="F44" s="6" t="s">
         <v>309</v>
       </c>
+      <c r="G44" t="s" s="0">
+        <v>718</v>
+      </c>
       <c r="H44" t="s" s="0">
         <v>550</v>
       </c>
@@ -3667,6 +4369,9 @@
       </c>
       <c r="J44" s="3" t="s">
         <v>172</v>
+      </c>
+      <c r="K44" t="s">
+        <v>717</v>
       </c>
       <c r="L44" s="0">
         <v>0</v>
@@ -3691,6 +4396,9 @@
       <c r="F45" s="6" t="s">
         <v>310</v>
       </c>
+      <c r="G45" t="s" s="0">
+        <v>720</v>
+      </c>
       <c r="H45" t="s" s="0">
         <v>550</v>
       </c>
@@ -3699,6 +4407,9 @@
       </c>
       <c r="J45" s="3" t="s">
         <v>173</v>
+      </c>
+      <c r="K45" t="s">
+        <v>719</v>
       </c>
       <c r="L45" s="0">
         <v>0</v>
@@ -3723,6 +4434,9 @@
       <c r="F46" s="6" t="s">
         <v>311</v>
       </c>
+      <c r="G46" t="s" s="0">
+        <v>722</v>
+      </c>
       <c r="H46" t="s" s="0">
         <v>550</v>
       </c>
@@ -3731,6 +4445,9 @@
       </c>
       <c r="J46" s="3" t="s">
         <v>174</v>
+      </c>
+      <c r="K46" t="s">
+        <v>721</v>
       </c>
       <c r="L46" s="0">
         <v>0</v>
@@ -3755,6 +4472,9 @@
       <c r="F47" s="6" t="s">
         <v>312</v>
       </c>
+      <c r="G47" t="s" s="0">
+        <v>724</v>
+      </c>
       <c r="H47" t="s" s="0">
         <v>550</v>
       </c>
@@ -3763,6 +4483,9 @@
       </c>
       <c r="J47" s="3" t="s">
         <v>175</v>
+      </c>
+      <c r="K47" t="s">
+        <v>723</v>
       </c>
       <c r="L47" s="0">
         <v>0</v>
@@ -3787,6 +4510,9 @@
       <c r="F48" s="6" t="s">
         <v>297</v>
       </c>
+      <c r="G48" t="s" s="0">
+        <v>725</v>
+      </c>
       <c r="H48" t="s" s="0">
         <v>550</v>
       </c>
@@ -3795,6 +4521,9 @@
       </c>
       <c r="J48" s="3" t="s">
         <v>155</v>
+      </c>
+      <c r="K48" t="s">
+        <v>683</v>
       </c>
       <c r="L48" s="0">
         <v>0</v>
@@ -3819,6 +4548,9 @@
       <c r="F49" s="6" t="s">
         <v>313</v>
       </c>
+      <c r="G49" t="s" s="0">
+        <v>727</v>
+      </c>
       <c r="H49" t="s" s="0">
         <v>550</v>
       </c>
@@ -3827,6 +4559,9 @@
       </c>
       <c r="J49" s="3" t="s">
         <v>176</v>
+      </c>
+      <c r="K49" t="s">
+        <v>726</v>
       </c>
       <c r="L49" s="0">
         <v>0</v>
@@ -3851,6 +4586,9 @@
       <c r="F50" s="6" t="s">
         <v>304</v>
       </c>
+      <c r="G50" t="s" s="0">
+        <v>729</v>
+      </c>
       <c r="H50" t="s" s="0">
         <v>550</v>
       </c>
@@ -3859,6 +4597,9 @@
       </c>
       <c r="J50" s="3" t="s">
         <v>177</v>
+      </c>
+      <c r="K50" t="s">
+        <v>728</v>
       </c>
       <c r="L50" s="0">
         <v>0</v>
@@ -3883,6 +4624,9 @@
       <c r="F51" s="6" t="s">
         <v>291</v>
       </c>
+      <c r="G51" t="s" s="0">
+        <v>731</v>
+      </c>
       <c r="H51" t="s" s="0">
         <v>550</v>
       </c>
@@ -3891,6 +4635,9 @@
       </c>
       <c r="J51" s="3" t="s">
         <v>178</v>
+      </c>
+      <c r="K51" t="s">
+        <v>730</v>
       </c>
       <c r="L51" s="0">
         <v>0</v>
@@ -3915,6 +4662,9 @@
       <c r="F52" s="6" t="s">
         <v>304</v>
       </c>
+      <c r="G52" t="s" s="0">
+        <v>733</v>
+      </c>
       <c r="H52" t="s" s="0">
         <v>550</v>
       </c>
@@ -3923,6 +4673,9 @@
       </c>
       <c r="J52" s="3" t="s">
         <v>179</v>
+      </c>
+      <c r="K52" t="s">
+        <v>732</v>
       </c>
       <c r="L52" s="0">
         <v>0</v>
@@ -3947,6 +4700,9 @@
       <c r="F53" s="6" t="s">
         <v>304</v>
       </c>
+      <c r="G53" t="s" s="0">
+        <v>735</v>
+      </c>
       <c r="H53" t="s" s="0">
         <v>550</v>
       </c>
@@ -3955,6 +4711,9 @@
       </c>
       <c r="J53" s="3" t="s">
         <v>180</v>
+      </c>
+      <c r="K53" t="s">
+        <v>734</v>
       </c>
       <c r="L53" s="0">
         <v>0</v>
@@ -3979,6 +4738,9 @@
       <c r="F54" s="6" t="s">
         <v>314</v>
       </c>
+      <c r="G54" t="s" s="0">
+        <v>737</v>
+      </c>
       <c r="H54" t="s" s="0">
         <v>550</v>
       </c>
@@ -3987,6 +4749,9 @@
       </c>
       <c r="J54" s="3" t="s">
         <v>181</v>
+      </c>
+      <c r="K54" t="s">
+        <v>736</v>
       </c>
       <c r="L54" s="0">
         <v>0</v>
@@ -4011,6 +4776,9 @@
       <c r="F55" s="6" t="s">
         <v>314</v>
       </c>
+      <c r="G55" t="s" s="0">
+        <v>739</v>
+      </c>
       <c r="H55" t="s" s="0">
         <v>550</v>
       </c>
@@ -4019,6 +4787,9 @@
       </c>
       <c r="J55" s="3" t="s">
         <v>182</v>
+      </c>
+      <c r="K55" t="s">
+        <v>738</v>
       </c>
       <c r="L55" s="0">
         <v>0</v>
@@ -4067,6 +4838,9 @@
       <c r="F60" s="6" t="s">
         <v>301</v>
       </c>
+      <c r="G60" t="s" s="0">
+        <v>741</v>
+      </c>
       <c r="H60" t="s" s="0">
         <v>550</v>
       </c>
@@ -4075,6 +4849,9 @@
       </c>
       <c r="J60" s="3" t="s">
         <v>183</v>
+      </c>
+      <c r="K60" t="s">
+        <v>740</v>
       </c>
       <c r="L60" s="0">
         <v>0</v>
@@ -4099,6 +4876,9 @@
       <c r="F61" s="6" t="s">
         <v>316</v>
       </c>
+      <c r="G61" t="s" s="0">
+        <v>743</v>
+      </c>
       <c r="H61" t="s" s="0">
         <v>550</v>
       </c>
@@ -4107,6 +4887,9 @@
       </c>
       <c r="J61" s="3" t="s">
         <v>184</v>
+      </c>
+      <c r="K61" t="s">
+        <v>742</v>
       </c>
       <c r="L61" s="0">
         <v>0</v>
@@ -4131,6 +4914,9 @@
       <c r="F62" s="6" t="s">
         <v>301</v>
       </c>
+      <c r="G62" t="s" s="0">
+        <v>745</v>
+      </c>
       <c r="H62" t="s" s="0">
         <v>550</v>
       </c>
@@ -4139,6 +4925,9 @@
       </c>
       <c r="J62" s="3" t="s">
         <v>185</v>
+      </c>
+      <c r="K62" t="s">
+        <v>744</v>
       </c>
       <c r="L62" s="0">
         <v>0</v>
@@ -4163,6 +4952,9 @@
       <c r="F63" s="6" t="s">
         <v>294</v>
       </c>
+      <c r="G63" t="s" s="0">
+        <v>747</v>
+      </c>
       <c r="H63" t="s" s="0">
         <v>550</v>
       </c>
@@ -4171,6 +4963,9 @@
       </c>
       <c r="J63" s="3" t="s">
         <v>186</v>
+      </c>
+      <c r="K63" t="s">
+        <v>746</v>
       </c>
       <c r="L63" s="0">
         <v>0</v>
@@ -4195,6 +4990,9 @@
       <c r="F64" s="6" t="s">
         <v>314</v>
       </c>
+      <c r="G64" t="s" s="0">
+        <v>749</v>
+      </c>
       <c r="H64" t="s" s="0">
         <v>550</v>
       </c>
@@ -4203,6 +5001,9 @@
       </c>
       <c r="J64" s="3" t="s">
         <v>187</v>
+      </c>
+      <c r="K64" t="s">
+        <v>748</v>
       </c>
       <c r="L64" s="0">
         <v>0</v>
@@ -4227,6 +5028,9 @@
       <c r="F65" s="6" t="s">
         <v>303</v>
       </c>
+      <c r="G65" t="s" s="0">
+        <v>751</v>
+      </c>
       <c r="H65" t="s" s="0">
         <v>550</v>
       </c>
@@ -4235,6 +5039,9 @@
       </c>
       <c r="J65" s="3" t="s">
         <v>188</v>
+      </c>
+      <c r="K65" t="s">
+        <v>750</v>
       </c>
       <c r="L65" s="0">
         <v>0</v>
@@ -4259,6 +5066,9 @@
       <c r="F66" s="6" t="s">
         <v>301</v>
       </c>
+      <c r="G66" t="s" s="0">
+        <v>753</v>
+      </c>
       <c r="H66" t="s" s="0">
         <v>550</v>
       </c>
@@ -4267,6 +5077,9 @@
       </c>
       <c r="J66" s="3" t="s">
         <v>189</v>
+      </c>
+      <c r="K66" t="s">
+        <v>752</v>
       </c>
       <c r="L66" s="0">
         <v>0</v>
@@ -4291,6 +5104,9 @@
       <c r="F67" s="6" t="s">
         <v>297</v>
       </c>
+      <c r="G67" t="s" s="0">
+        <v>755</v>
+      </c>
       <c r="H67" t="s" s="0">
         <v>550</v>
       </c>
@@ -4299,6 +5115,9 @@
       </c>
       <c r="J67" s="3" t="s">
         <v>190</v>
+      </c>
+      <c r="K67" t="s">
+        <v>754</v>
       </c>
       <c r="L67" s="0">
         <v>0</v>
@@ -4323,6 +5142,9 @@
       <c r="F68" s="6" t="s">
         <v>294</v>
       </c>
+      <c r="G68" t="s" s="0">
+        <v>757</v>
+      </c>
       <c r="H68" t="s" s="0">
         <v>550</v>
       </c>
@@ -4331,6 +5153,9 @@
       </c>
       <c r="J68" s="3" t="s">
         <v>191</v>
+      </c>
+      <c r="K68" t="s">
+        <v>756</v>
       </c>
       <c r="L68" s="0">
         <v>0</v>
@@ -4355,6 +5180,9 @@
       <c r="F69" s="6" t="s">
         <v>317</v>
       </c>
+      <c r="G69" t="s" s="0">
+        <v>759</v>
+      </c>
       <c r="H69" t="s" s="0">
         <v>550</v>
       </c>
@@ -4363,6 +5191,9 @@
       </c>
       <c r="J69" s="3" t="s">
         <v>192</v>
+      </c>
+      <c r="K69" t="s">
+        <v>758</v>
       </c>
       <c r="L69" s="0">
         <v>0</v>
@@ -4387,6 +5218,9 @@
       <c r="F70" s="6" t="s">
         <v>314</v>
       </c>
+      <c r="G70" t="s" s="0">
+        <v>761</v>
+      </c>
       <c r="H70" t="s" s="0">
         <v>550</v>
       </c>
@@ -4395,6 +5229,9 @@
       </c>
       <c r="J70" s="3" t="s">
         <v>193</v>
+      </c>
+      <c r="K70" t="s">
+        <v>760</v>
       </c>
       <c r="L70" s="0">
         <v>0</v>
@@ -4419,6 +5256,9 @@
       <c r="F71" s="6" t="s">
         <v>301</v>
       </c>
+      <c r="G71" t="s" s="0">
+        <v>762</v>
+      </c>
       <c r="H71" t="s" s="0">
         <v>550</v>
       </c>
@@ -4427,6 +5267,9 @@
       </c>
       <c r="J71" s="3" t="s">
         <v>183</v>
+      </c>
+      <c r="K71" t="s">
+        <v>740</v>
       </c>
       <c r="L71" s="0">
         <v>0</v>
@@ -4451,6 +5294,9 @@
       <c r="F72" s="6" t="s">
         <v>314</v>
       </c>
+      <c r="G72" t="s" s="0">
+        <v>764</v>
+      </c>
       <c r="H72" t="s" s="0">
         <v>550</v>
       </c>
@@ -4459,6 +5305,9 @@
       </c>
       <c r="J72" s="3" t="s">
         <v>194</v>
+      </c>
+      <c r="K72" t="s">
+        <v>763</v>
       </c>
       <c r="L72" s="0">
         <v>0</v>
@@ -4483,6 +5332,9 @@
       <c r="F73" s="6" t="s">
         <v>294</v>
       </c>
+      <c r="G73" t="s" s="0">
+        <v>766</v>
+      </c>
       <c r="H73" t="s" s="0">
         <v>550</v>
       </c>
@@ -4491,6 +5343,9 @@
       </c>
       <c r="J73" s="3" t="s">
         <v>195</v>
+      </c>
+      <c r="K73" t="s">
+        <v>765</v>
       </c>
       <c r="L73" s="0">
         <v>0</v>
@@ -4515,6 +5370,9 @@
       <c r="F74" s="6" t="s">
         <v>300</v>
       </c>
+      <c r="G74" t="s" s="0">
+        <v>768</v>
+      </c>
       <c r="H74" t="s" s="0">
         <v>550</v>
       </c>
@@ -4523,6 +5381,9 @@
       </c>
       <c r="J74" s="3" t="s">
         <v>196</v>
+      </c>
+      <c r="K74" t="s">
+        <v>767</v>
       </c>
       <c r="L74" s="0">
         <v>0</v>
@@ -4547,6 +5408,9 @@
       <c r="F75" s="6" t="s">
         <v>291</v>
       </c>
+      <c r="G75" t="s" s="0">
+        <v>770</v>
+      </c>
       <c r="H75" t="s" s="0">
         <v>550</v>
       </c>
@@ -4555,6 +5419,9 @@
       </c>
       <c r="J75" s="3" t="s">
         <v>197</v>
+      </c>
+      <c r="K75" t="s">
+        <v>769</v>
       </c>
       <c r="L75" s="0">
         <v>0</v>
@@ -4579,6 +5446,9 @@
       <c r="F76" s="6" t="s">
         <v>301</v>
       </c>
+      <c r="G76" t="s" s="0">
+        <v>772</v>
+      </c>
       <c r="H76" t="s" s="0">
         <v>550</v>
       </c>
@@ -4587,6 +5457,9 @@
       </c>
       <c r="J76" s="3" t="s">
         <v>198</v>
+      </c>
+      <c r="K76" t="s">
+        <v>771</v>
       </c>
       <c r="L76" s="0">
         <v>0</v>
@@ -4611,6 +5484,9 @@
       <c r="F77" s="6" t="s">
         <v>301</v>
       </c>
+      <c r="G77" t="s" s="0">
+        <v>774</v>
+      </c>
       <c r="H77" t="s" s="0">
         <v>550</v>
       </c>
@@ -4619,6 +5495,9 @@
       </c>
       <c r="J77" s="3" t="s">
         <v>638</v>
+      </c>
+      <c r="K77" t="s">
+        <v>773</v>
       </c>
       <c r="L77" s="0">
         <v>0</v>
@@ -4649,6 +5528,9 @@
       <c r="F79" s="6" t="s">
         <v>297</v>
       </c>
+      <c r="G79" t="s" s="0">
+        <v>776</v>
+      </c>
       <c r="H79" t="s" s="0">
         <v>550</v>
       </c>
@@ -4657,6 +5539,9 @@
       </c>
       <c r="J79" s="3" t="s">
         <v>199</v>
+      </c>
+      <c r="K79" t="s">
+        <v>775</v>
       </c>
       <c r="L79" s="0">
         <v>0</v>
@@ -4681,6 +5566,9 @@
       <c r="F80" s="6" t="s">
         <v>319</v>
       </c>
+      <c r="G80" t="s" s="0">
+        <v>778</v>
+      </c>
       <c r="H80" t="s" s="0">
         <v>550</v>
       </c>
@@ -4689,6 +5577,9 @@
       </c>
       <c r="J80" s="3" t="s">
         <v>639</v>
+      </c>
+      <c r="K80" t="s">
+        <v>777</v>
       </c>
       <c r="L80" s="0">
         <v>0</v>
@@ -4713,6 +5604,9 @@
       <c r="F81" s="6" t="s">
         <v>297</v>
       </c>
+      <c r="G81" t="s" s="0">
+        <v>780</v>
+      </c>
       <c r="H81" t="s" s="0">
         <v>550</v>
       </c>
@@ -4721,6 +5615,9 @@
       </c>
       <c r="J81" s="3" t="s">
         <v>200</v>
+      </c>
+      <c r="K81" t="s">
+        <v>779</v>
       </c>
       <c r="L81" s="0">
         <v>0</v>
@@ -4745,6 +5642,9 @@
       <c r="F82" s="6" t="s">
         <v>320</v>
       </c>
+      <c r="G82" t="s" s="0">
+        <v>782</v>
+      </c>
       <c r="H82" t="s" s="0">
         <v>550</v>
       </c>
@@ -4753,6 +5653,9 @@
       </c>
       <c r="J82" s="3" t="s">
         <v>201</v>
+      </c>
+      <c r="K82" t="s">
+        <v>781</v>
       </c>
       <c r="L82" s="0">
         <v>0</v>
@@ -4777,6 +5680,9 @@
       <c r="F83" s="6" t="s">
         <v>314</v>
       </c>
+      <c r="G83" t="s" s="0">
+        <v>784</v>
+      </c>
       <c r="H83" t="s" s="0">
         <v>550</v>
       </c>
@@ -4785,6 +5691,9 @@
       </c>
       <c r="J83" s="3" t="s">
         <v>640</v>
+      </c>
+      <c r="K83" t="s">
+        <v>783</v>
       </c>
       <c r="L83" s="0">
         <v>0</v>
@@ -4809,6 +5718,9 @@
       <c r="F84" s="6" t="s">
         <v>315</v>
       </c>
+      <c r="G84" t="s" s="0">
+        <v>786</v>
+      </c>
       <c r="H84" t="s" s="0">
         <v>550</v>
       </c>
@@ -4817,6 +5729,9 @@
       </c>
       <c r="J84" s="3" t="s">
         <v>202</v>
+      </c>
+      <c r="K84" t="s">
+        <v>785</v>
       </c>
       <c r="L84" s="0">
         <v>0</v>
@@ -4847,6 +5762,9 @@
       <c r="F86" s="6" t="s">
         <v>304</v>
       </c>
+      <c r="G86" t="s" s="0">
+        <v>788</v>
+      </c>
       <c r="H86" t="s" s="0">
         <v>550</v>
       </c>
@@ -4855,6 +5773,9 @@
       </c>
       <c r="J86" s="3" t="s">
         <v>203</v>
+      </c>
+      <c r="K86" t="s">
+        <v>787</v>
       </c>
       <c r="L86" s="0">
         <v>0</v>
@@ -4879,6 +5800,9 @@
       <c r="F87" s="6" t="s">
         <v>304</v>
       </c>
+      <c r="G87" t="s" s="0">
+        <v>790</v>
+      </c>
       <c r="H87" t="s" s="0">
         <v>550</v>
       </c>
@@ -4887,6 +5811,9 @@
       </c>
       <c r="J87" s="3" t="s">
         <v>204</v>
+      </c>
+      <c r="K87" t="s">
+        <v>789</v>
       </c>
       <c r="L87" s="0">
         <v>0</v>
@@ -4911,6 +5838,9 @@
       <c r="F88" s="6" t="s">
         <v>295</v>
       </c>
+      <c r="G88" t="s" s="0">
+        <v>792</v>
+      </c>
       <c r="H88" t="s" s="0">
         <v>550</v>
       </c>
@@ -4919,6 +5849,9 @@
       </c>
       <c r="J88" s="3" t="s">
         <v>205</v>
+      </c>
+      <c r="K88" t="s">
+        <v>791</v>
       </c>
       <c r="L88" s="0">
         <v>0</v>
@@ -4943,6 +5876,9 @@
       <c r="F89" s="6" t="s">
         <v>295</v>
       </c>
+      <c r="G89" t="s" s="0">
+        <v>794</v>
+      </c>
       <c r="H89" t="s" s="0">
         <v>550</v>
       </c>
@@ -4951,6 +5887,9 @@
       </c>
       <c r="J89" s="3" t="s">
         <v>206</v>
+      </c>
+      <c r="K89" t="s">
+        <v>793</v>
       </c>
       <c r="L89" s="0">
         <v>0</v>
@@ -4975,6 +5914,9 @@
       <c r="F90" s="6" t="s">
         <v>321</v>
       </c>
+      <c r="G90" t="s" s="0">
+        <v>796</v>
+      </c>
       <c r="H90" t="s" s="0">
         <v>550</v>
       </c>
@@ -4983,6 +5925,9 @@
       </c>
       <c r="J90" s="3" t="s">
         <v>207</v>
+      </c>
+      <c r="K90" t="s">
+        <v>795</v>
       </c>
       <c r="L90" s="0">
         <v>0</v>
@@ -5007,6 +5952,9 @@
       <c r="F91" s="6" t="s">
         <v>301</v>
       </c>
+      <c r="G91" t="s" s="0">
+        <v>798</v>
+      </c>
       <c r="H91" t="s" s="0">
         <v>550</v>
       </c>
@@ -5015,6 +5963,9 @@
       </c>
       <c r="J91" s="3" t="s">
         <v>208</v>
+      </c>
+      <c r="K91" t="s">
+        <v>797</v>
       </c>
       <c r="L91" s="0">
         <v>0</v>
@@ -5039,6 +5990,9 @@
       <c r="F92" s="6" t="s">
         <v>322</v>
       </c>
+      <c r="G92" t="s" s="0">
+        <v>800</v>
+      </c>
       <c r="H92" t="s" s="0">
         <v>550</v>
       </c>
@@ -5047,6 +6001,9 @@
       </c>
       <c r="J92" s="3" t="s">
         <v>209</v>
+      </c>
+      <c r="K92" t="s">
+        <v>799</v>
       </c>
       <c r="L92" s="0">
         <v>0</v>
@@ -5071,6 +6028,9 @@
       <c r="F93" s="6" t="s">
         <v>305</v>
       </c>
+      <c r="G93" t="s" s="0">
+        <v>802</v>
+      </c>
       <c r="H93" t="s" s="0">
         <v>550</v>
       </c>
@@ -5079,6 +6039,9 @@
       </c>
       <c r="J93" s="3" t="s">
         <v>210</v>
+      </c>
+      <c r="K93" t="s">
+        <v>801</v>
       </c>
       <c r="L93" s="0">
         <v>0</v>
@@ -5103,6 +6066,9 @@
       <c r="F94" s="6" t="s">
         <v>323</v>
       </c>
+      <c r="G94" t="s" s="0">
+        <v>804</v>
+      </c>
       <c r="H94" t="s" s="0">
         <v>550</v>
       </c>
@@ -5111,6 +6077,9 @@
       </c>
       <c r="J94" s="3" t="s">
         <v>211</v>
+      </c>
+      <c r="K94" t="s">
+        <v>803</v>
       </c>
       <c r="L94" s="0">
         <v>0</v>
@@ -5135,6 +6104,9 @@
       <c r="F95" s="6" t="s">
         <v>298</v>
       </c>
+      <c r="G95" t="s" s="0">
+        <v>806</v>
+      </c>
       <c r="H95" t="s" s="0">
         <v>550</v>
       </c>
@@ -5143,6 +6115,9 @@
       </c>
       <c r="J95" s="3" t="s">
         <v>212</v>
+      </c>
+      <c r="K95" t="s">
+        <v>805</v>
       </c>
       <c r="L95" s="0">
         <v>0</v>
@@ -5202,6 +6177,9 @@
       <c r="F102" s="6" t="s">
         <v>325</v>
       </c>
+      <c r="G102" t="s" s="0">
+        <v>808</v>
+      </c>
       <c r="H102" t="s" s="0">
         <v>550</v>
       </c>
@@ -5210,6 +6188,9 @@
       </c>
       <c r="J102" s="3" t="s">
         <v>641</v>
+      </c>
+      <c r="K102" t="s">
+        <v>807</v>
       </c>
       <c r="L102" s="0">
         <v>0</v>
@@ -5234,6 +6215,9 @@
       <c r="F103" s="6" t="s">
         <v>292</v>
       </c>
+      <c r="G103" t="s" s="0">
+        <v>810</v>
+      </c>
       <c r="H103" t="s" s="0">
         <v>550</v>
       </c>
@@ -5242,6 +6226,9 @@
       </c>
       <c r="J103" s="3" t="s">
         <v>642</v>
+      </c>
+      <c r="K103" t="s">
+        <v>809</v>
       </c>
       <c r="L103" s="0">
         <v>0</v>
@@ -5266,6 +6253,9 @@
       <c r="F104" s="6" t="s">
         <v>290</v>
       </c>
+      <c r="G104" t="s" s="0">
+        <v>812</v>
+      </c>
       <c r="H104" t="s" s="0">
         <v>550</v>
       </c>
@@ -5274,6 +6264,9 @@
       </c>
       <c r="J104" s="3" t="s">
         <v>213</v>
+      </c>
+      <c r="K104" t="s">
+        <v>811</v>
       </c>
       <c r="L104" s="0">
         <v>0</v>
@@ -5298,6 +6291,9 @@
       <c r="F105" s="6" t="s">
         <v>314</v>
       </c>
+      <c r="G105" t="s" s="0">
+        <v>814</v>
+      </c>
       <c r="H105" t="s" s="0">
         <v>550</v>
       </c>
@@ -5306,6 +6302,9 @@
       </c>
       <c r="J105" s="3" t="s">
         <v>214</v>
+      </c>
+      <c r="K105" t="s">
+        <v>813</v>
       </c>
       <c r="L105" s="0">
         <v>0</v>
@@ -5330,6 +6329,9 @@
       <c r="F106" s="6" t="s">
         <v>314</v>
       </c>
+      <c r="G106" t="s" s="0">
+        <v>816</v>
+      </c>
       <c r="H106" t="s" s="0">
         <v>550</v>
       </c>
@@ -5338,6 +6340,9 @@
       </c>
       <c r="J106" s="3" t="s">
         <v>643</v>
+      </c>
+      <c r="K106" t="s">
+        <v>815</v>
       </c>
       <c r="L106" s="0">
         <v>0</v>
@@ -5462,6 +6467,9 @@
       <c r="F127" s="6" t="s">
         <v>326</v>
       </c>
+      <c r="G127" t="s" s="0">
+        <v>818</v>
+      </c>
       <c r="H127" t="s" s="0">
         <v>550</v>
       </c>
@@ -5472,7 +6480,7 @@
         <v>215</v>
       </c>
       <c r="K127" t="s" s="0">
-        <v>647</v>
+        <v>817</v>
       </c>
       <c r="L127" s="0">
         <v>0</v>
@@ -5497,6 +6505,9 @@
       <c r="F128" s="6" t="s">
         <v>327</v>
       </c>
+      <c r="G128" t="s" s="0">
+        <v>820</v>
+      </c>
       <c r="H128" t="s" s="0">
         <v>550</v>
       </c>
@@ -5507,7 +6518,7 @@
         <v>644</v>
       </c>
       <c r="K128" t="s" s="0">
-        <v>648</v>
+        <v>819</v>
       </c>
       <c r="L128" s="0">
         <v>0</v>
@@ -5532,6 +6543,9 @@
       <c r="F129" s="6" t="s">
         <v>318</v>
       </c>
+      <c r="G129" t="s" s="0">
+        <v>821</v>
+      </c>
       <c r="H129" t="s" s="0">
         <v>550</v>
       </c>
@@ -5567,6 +6581,9 @@
       <c r="F130" s="6" t="s">
         <v>294</v>
       </c>
+      <c r="G130" t="s" s="0">
+        <v>822</v>
+      </c>
       <c r="H130" t="s" s="0">
         <v>550</v>
       </c>
@@ -5602,6 +6619,9 @@
       <c r="F131" s="6" t="s">
         <v>324</v>
       </c>
+      <c r="G131" t="s" s="0">
+        <v>823</v>
+      </c>
       <c r="H131" t="s" s="0">
         <v>550</v>
       </c>
@@ -5637,6 +6657,9 @@
       <c r="F132" s="6" t="s">
         <v>324</v>
       </c>
+      <c r="G132" t="s" s="0">
+        <v>824</v>
+      </c>
       <c r="H132" t="s" s="0">
         <v>550</v>
       </c>
@@ -5672,6 +6695,9 @@
       <c r="F133" s="6" t="s">
         <v>322</v>
       </c>
+      <c r="G133" t="s" s="0">
+        <v>825</v>
+      </c>
       <c r="H133" t="s" s="0">
         <v>550</v>
       </c>
@@ -5707,6 +6733,9 @@
       <c r="F134" s="6" t="s">
         <v>328</v>
       </c>
+      <c r="G134" t="s" s="0">
+        <v>826</v>
+      </c>
       <c r="H134" t="s" s="0">
         <v>550</v>
       </c>
@@ -5742,6 +6771,9 @@
       <c r="F135" s="6" t="s">
         <v>318</v>
       </c>
+      <c r="G135" t="s" s="0">
+        <v>828</v>
+      </c>
       <c r="H135" t="s" s="0">
         <v>550</v>
       </c>
@@ -5752,7 +6784,7 @@
         <v>222</v>
       </c>
       <c r="K135" t="s" s="0">
-        <v>655</v>
+        <v>827</v>
       </c>
       <c r="L135" s="0">
         <v>0</v>
@@ -5777,6 +6809,9 @@
       <c r="F136" s="6" t="s">
         <v>297</v>
       </c>
+      <c r="G136" t="s" s="0">
+        <v>830</v>
+      </c>
       <c r="H136" t="s" s="0">
         <v>550</v>
       </c>
@@ -5787,7 +6822,7 @@
         <v>223</v>
       </c>
       <c r="K136" t="s" s="0">
-        <v>656</v>
+        <v>829</v>
       </c>
       <c r="L136" s="0">
         <v>0</v>

</xml_diff>